<commit_message>
updated with bug magnet
</commit_message>
<xml_diff>
--- a/Test_Cases/Capstone_Test_Cases.xlsx
+++ b/Test_Cases/Capstone_Test_Cases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jferg\Class12Capstone\Test_Cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DED2D31B-EAD1-45BB-A6F6-32EAD62FAB7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF6D82CD-8E84-4058-8674-08F54387C799}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33720" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AC1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="101">
   <si>
     <t>Test Steps</t>
   </si>
@@ -114,9 +114,6 @@
     <t>New Veternarian will appear</t>
   </si>
   <si>
-    <t>Add First Name= John  Last Name = Doe</t>
-  </si>
-  <si>
     <t>Click Save Vet</t>
   </si>
   <si>
@@ -129,9 +126,6 @@
     <t>Click OWNERS dropdown and click add new</t>
   </si>
   <si>
-    <t>Add First Name= John  Last Name = Doe  Address= 123  City= tyler  Telephone= 1231231234</t>
-  </si>
-  <si>
     <t>Click Add Owner</t>
   </si>
   <si>
@@ -334,6 +328,9 @@
   </si>
   <si>
     <t>Type wont be allowed to be entered</t>
+  </si>
+  <si>
+    <t>Right click each section and select bug magnet to input data</t>
   </si>
 </sst>
 </file>
@@ -822,8 +819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:E46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -837,7 +834,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -918,7 +915,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>14</v>
@@ -986,7 +983,7 @@
         <v>11</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>14</v>
@@ -1054,7 +1051,7 @@
         <v>12</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>14</v>
@@ -1113,10 +1110,10 @@
     </row>
     <row r="27" spans="1:5" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C27" s="9" t="s">
         <v>14</v>
@@ -1127,10 +1124,10 @@
     <row r="28" spans="1:5" ht="59" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="10"/>
       <c r="B28" s="11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D28" s="10"/>
       <c r="E28" s="10"/>
@@ -1138,10 +1135,10 @@
     <row r="29" spans="1:5" ht="35.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="12"/>
       <c r="B29" s="11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D29" s="10"/>
       <c r="E29" s="10"/>
@@ -1149,10 +1146,10 @@
     <row r="30" spans="1:5" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="10"/>
       <c r="B30" s="11" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D30" s="10"/>
       <c r="E30" s="10"/>
@@ -1160,10 +1157,10 @@
     <row r="31" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="10"/>
       <c r="B31" s="11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D31" s="10"/>
       <c r="E31" s="10"/>
@@ -1171,10 +1168,10 @@
     <row r="32" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="10"/>
       <c r="B32" s="11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D32" s="10"/>
       <c r="E32" s="10"/>
@@ -1182,10 +1179,10 @@
     <row r="33" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="10"/>
       <c r="B33" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D33" s="10"/>
       <c r="E33" s="10"/>
@@ -1193,24 +1190,24 @@
     <row r="34" spans="1:8" ht="41.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="10"/>
       <c r="B34" s="11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D34" s="10"/>
       <c r="E34" s="10"/>
       <c r="H34" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="10"/>
       <c r="B35" s="11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D35" s="10"/>
       <c r="E35" s="10"/>
@@ -1218,10 +1215,10 @@
     <row r="36" spans="1:8" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A36" s="10"/>
       <c r="B36" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D36" s="10"/>
       <c r="E36" s="10"/>
@@ -1252,10 +1249,10 @@
     </row>
     <row r="39" spans="1:8" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C39" s="9" t="s">
         <v>14</v>
@@ -1266,10 +1263,10 @@
     <row r="40" spans="1:8" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="10"/>
       <c r="B40" s="11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D40" s="10"/>
       <c r="E40" s="10"/>
@@ -1277,10 +1274,10 @@
     <row r="41" spans="1:8" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41" s="12"/>
       <c r="B41" s="11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D41" s="10"/>
       <c r="E41" s="10"/>
@@ -1288,10 +1285,10 @@
     <row r="42" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A42" s="10"/>
       <c r="B42" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D42" s="10"/>
       <c r="E42" s="10"/>
@@ -1299,10 +1296,10 @@
     <row r="43" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A43" s="10"/>
       <c r="B43" s="11" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D43" s="10"/>
       <c r="E43" s="10"/>
@@ -1310,10 +1307,10 @@
     <row r="44" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A44" s="10"/>
       <c r="B44" s="11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D44" s="10"/>
       <c r="E44" s="10"/>
@@ -1321,10 +1318,10 @@
     <row r="45" spans="1:8" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A45" s="10"/>
       <c r="B45" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D45" s="10"/>
       <c r="E45" s="10"/>
@@ -1332,10 +1329,10 @@
     <row r="46" spans="1:8" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A46" s="10"/>
       <c r="B46" s="11" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D46" s="10"/>
       <c r="E46" s="10"/>
@@ -1350,8 +1347,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9763E1BE-D17A-4D71-98A6-15FEBD47A28F}">
   <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:E45"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1364,7 +1361,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -1445,7 +1442,7 @@
         <v>25</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>14</v>
@@ -1498,7 +1495,7 @@
     <row r="14" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="10"/>
       <c r="B14" s="11" t="s">
-        <v>28</v>
+        <v>100</v>
       </c>
       <c r="C14" s="11"/>
       <c r="D14" s="10"/>
@@ -1507,10 +1504,10 @@
     <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="12"/>
       <c r="B15" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="11" t="s">
         <v>29</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>30</v>
       </c>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
@@ -1541,10 +1538,10 @@
     </row>
     <row r="18" spans="1:5" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>14</v>
@@ -1586,7 +1583,7 @@
     <row r="22" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="12"/>
       <c r="B22" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C22" s="11" t="s">
         <v>27</v>
@@ -1594,10 +1591,10 @@
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
     </row>
-    <row r="23" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="10"/>
       <c r="B23" s="11" t="s">
-        <v>33</v>
+        <v>100</v>
       </c>
       <c r="C23" s="11"/>
       <c r="D23" s="10"/>
@@ -1606,10 +1603,10 @@
     <row r="24" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="12"/>
       <c r="B24" s="11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>
@@ -1617,7 +1614,7 @@
     <row r="25" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="26" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>0</v>
@@ -1634,10 +1631,10 @@
     </row>
     <row r="27" spans="1:5" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C27" s="9" t="s">
         <v>14</v>
@@ -1648,7 +1645,7 @@
     <row r="28" spans="1:5" ht="73" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="10"/>
       <c r="B28" s="11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C28" s="11"/>
       <c r="D28" s="10"/>
@@ -1657,10 +1654,10 @@
     <row r="29" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="12"/>
       <c r="B29" s="11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D29" s="10"/>
       <c r="E29" s="10"/>
@@ -1668,10 +1665,10 @@
     <row r="30" spans="1:5" ht="35.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="10"/>
       <c r="B30" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D30" s="10"/>
       <c r="E30" s="10"/>
@@ -1679,10 +1676,10 @@
     <row r="31" spans="1:5" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="10"/>
       <c r="B31" s="11" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D31" s="10"/>
       <c r="E31" s="10"/>
@@ -1690,10 +1687,10 @@
     <row r="32" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="10"/>
       <c r="B32" s="11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D32" s="10"/>
       <c r="E32" s="10"/>
@@ -1701,10 +1698,10 @@
     <row r="33" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="10"/>
       <c r="B33" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D33" s="10"/>
       <c r="E33" s="10"/>
@@ -1742,7 +1739,7 @@
     </row>
     <row r="37" spans="1:5" ht="41" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B37" s="8" t="s">
         <v>13</v>
@@ -1756,7 +1753,7 @@
     <row r="38" spans="1:5" ht="73" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="10"/>
       <c r="B38" s="11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C38" s="11"/>
       <c r="D38" s="10"/>
@@ -1765,10 +1762,10 @@
     <row r="39" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="12"/>
       <c r="B39" s="11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D39" s="10"/>
       <c r="E39" s="10"/>
@@ -1776,10 +1773,10 @@
     <row r="40" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="10"/>
       <c r="B40" s="11" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D40" s="10"/>
       <c r="E40" s="10"/>
@@ -1787,10 +1784,10 @@
     <row r="41" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41" s="10"/>
       <c r="B41" s="11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D41" s="10"/>
       <c r="E41" s="10"/>
@@ -1798,10 +1795,10 @@
     <row r="42" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A42" s="10"/>
       <c r="B42" s="11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D42" s="10"/>
       <c r="E42" s="10"/>
@@ -1809,10 +1806,10 @@
     <row r="43" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A43" s="10"/>
       <c r="B43" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D43" s="10"/>
       <c r="E43" s="10"/>
@@ -1820,10 +1817,10 @@
     <row r="44" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A44" s="10"/>
       <c r="B44" s="11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D44" s="10"/>
       <c r="E44" s="10"/>
@@ -1831,10 +1828,10 @@
     <row r="45" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A45" s="10"/>
       <c r="B45" s="11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D45" s="10"/>
       <c r="E45" s="10"/>
@@ -1862,7 +1859,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -1940,10 +1937,10 @@
     </row>
     <row r="9" spans="1:5" ht="53.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>14</v>
@@ -1965,7 +1962,7 @@
     <row r="11" spans="1:5" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="12"/>
       <c r="B11" s="11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C11" s="11"/>
       <c r="D11" s="10"/>
@@ -1977,7 +1974,7 @@
         <v>18</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
@@ -2015,10 +2012,10 @@
     </row>
     <row r="16" spans="1:5" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>14</v>
@@ -2040,7 +2037,7 @@
     <row r="18" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="12"/>
       <c r="B18" s="11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C18" s="11"/>
       <c r="D18" s="10"/>
@@ -2052,10 +2049,10 @@
         <v>18</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E19" s="10"/>
     </row>
@@ -2082,7 +2079,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -2107,7 +2104,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -2116,7 +2113,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
@@ -2156,13 +2153,13 @@
     </row>
     <row r="9" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
@@ -2170,10 +2167,10 @@
     <row r="10" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="10"/>
       <c r="B10" s="11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
@@ -2181,7 +2178,7 @@
     <row r="11" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="10"/>
       <c r="B11" s="11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C11" s="11"/>
       <c r="D11" s="10"/>
@@ -2190,7 +2187,7 @@
     <row r="12" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="12"/>
       <c r="B12" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C12" s="11"/>
       <c r="D12" s="10"/>
@@ -2199,7 +2196,7 @@
     <row r="13" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="12"/>
       <c r="B13" s="11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C13" s="11"/>
       <c r="D13" s="10"/>
@@ -2208,10 +2205,10 @@
     <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="12"/>
       <c r="B14" s="11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
@@ -2219,7 +2216,7 @@
     <row r="15" spans="1:5" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="10"/>
       <c r="B15" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C15" s="11"/>
       <c r="D15" s="10"/>
@@ -2228,10 +2225,10 @@
     <row r="16" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="10"/>
       <c r="B16" s="11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>

</xml_diff>